<commit_message>
typed up kit requirements
</commit_message>
<xml_diff>
--- a/clutter/Product Specs.xlsx
+++ b/clutter/Product Specs.xlsx
@@ -8,14 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\myfiles\hrh33\dos\FYP Adjustabike\clutter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C42092C-E088-42B6-B1CC-AB9613073609}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0AA912C-9853-4302-B87A-FAA1D08A784C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-13110" yWindow="-240" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{0B1A8BE2-F423-4BD1-B9C4-448950125A23}"/>
+    <workbookView xWindow="-8655" yWindow="-300" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{0B1A8BE2-F423-4BD1-B9C4-448950125A23}"/>
   </bookViews>
   <sheets>
     <sheet name="bike" sheetId="1" r:id="rId1"/>
     <sheet name="kit" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">bike!$A$2:$D$45</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -32,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="80">
   <si>
     <t>D/W</t>
   </si>
@@ -203,6 +206,75 @@
   </si>
   <si>
     <t>Design can be either adapted (different parts) or adjusted to suit riders of * to * in height</t>
+  </si>
+  <si>
+    <t>links</t>
+  </si>
+  <si>
+    <t>joints</t>
+  </si>
+  <si>
+    <t>manufacture</t>
+  </si>
+  <si>
+    <t>Max weight/metre of *</t>
+  </si>
+  <si>
+    <t>The following lengths should be possible: * * *</t>
+  </si>
+  <si>
+    <t>Maximum cost of *</t>
+  </si>
+  <si>
+    <t>Minimise cost</t>
+  </si>
+  <si>
+    <t>The following angles should be possible: * * *</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Assemble securely </t>
+  </si>
+  <si>
+    <t>Possible to manufacture safely with only the tools available to a layman</t>
+  </si>
+  <si>
+    <t>Possible to manufacture with one person (can use vices to secure work)</t>
+  </si>
+  <si>
+    <t>Maximum manufacture time for basic kit: *</t>
+  </si>
+  <si>
+    <t>All components commercially available to a layman</t>
+  </si>
+  <si>
+    <t>Consistent/repeatable from documentation</t>
+  </si>
+  <si>
+    <t>other systems</t>
+  </si>
+  <si>
+    <t>Components for other systems (ie wheels, brakes, pedals, drive, steering, seat) selected to satisfy bike requirements</t>
+  </si>
+  <si>
+    <t>Attachment for other systems (ie wheels, brakes, pedals, drive, steering, seat) designed to satisfy bike requirements</t>
+  </si>
+  <si>
+    <t>All parts compatible</t>
+  </si>
+  <si>
+    <t>Minimum load of * in tension/compression and * bending</t>
+  </si>
+  <si>
+    <t>Minimum 'gripping' force of * and resistance to torque of *</t>
+  </si>
+  <si>
+    <t>Possibility of a different length without cutting link</t>
+  </si>
+  <si>
+    <t>Possibility of a different angle without using a different joint</t>
+  </si>
+  <si>
+    <t>"Standard" bike geometry and at least one other geometry possible</t>
   </si>
 </sst>
 </file>
@@ -253,11 +325,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -266,6 +335,24 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -584,325 +671,325 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78235AD6-7E08-4F88-97EC-47267900DBCA}">
   <dimension ref="A1:D45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B46" sqref="B46"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.140625" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.140625" customWidth="1"/>
     <col min="4" max="4" width="64.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-    </row>
-    <row r="2" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+    </row>
+    <row r="2" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>54</v>
+        <v>44</v>
+      </c>
+      <c r="B3" s="3">
+        <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="D3" t="s">
-        <v>4</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>44</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="3">
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="D4" t="s">
-        <v>5</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>46</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>54</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="D5" t="s">
-        <v>6</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>46</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>54</v>
+        <v>44</v>
+      </c>
+      <c r="B6" s="3">
+        <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="D6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>44</v>
-      </c>
-      <c r="B7" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>54</v>
       </c>
       <c r="C7" t="s">
-        <v>16</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>56</v>
+        <v>41</v>
+      </c>
+      <c r="D7" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>46</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="3" t="s">
         <v>54</v>
       </c>
       <c r="C8" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="D8" t="s">
-        <v>8</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>44</v>
       </c>
-      <c r="B9" s="4">
-        <v>1</v>
+      <c r="B9" s="3">
+        <v>5</v>
       </c>
       <c r="C9" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="D9" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>46</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="3" t="s">
         <v>54</v>
       </c>
       <c r="C10" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="D10" t="s">
-        <v>9</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>46</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="3" t="s">
         <v>54</v>
       </c>
       <c r="C11" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="D11" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>46</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="3" t="s">
         <v>54</v>
       </c>
       <c r="C12" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="D12" t="s">
-        <v>11</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>46</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="3" t="s">
         <v>54</v>
       </c>
       <c r="C13" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D13" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>44</v>
       </c>
-      <c r="B14" s="4">
-        <v>4</v>
+      <c r="B14" s="3">
+        <v>3</v>
       </c>
       <c r="C14" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D14" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>46</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="3" t="s">
         <v>54</v>
       </c>
       <c r="C15" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D15" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>46</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="3" t="s">
         <v>54</v>
       </c>
       <c r="C16" t="s">
         <v>16</v>
       </c>
       <c r="D16" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>46</v>
-      </c>
-      <c r="B17" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B17" s="3" t="s">
         <v>54</v>
       </c>
       <c r="C17" t="s">
-        <v>17</v>
-      </c>
-      <c r="D17" t="s">
-        <v>14</v>
+        <v>16</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>44</v>
-      </c>
-      <c r="B18" s="4">
-        <v>4</v>
+        <v>46</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>54</v>
       </c>
       <c r="C18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D18" t="s">
-        <v>55</v>
+        <v>8</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>44</v>
       </c>
-      <c r="B19" s="4">
-        <v>2</v>
+      <c r="B19" s="3">
+        <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>46</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B20" s="3" t="s">
         <v>54</v>
       </c>
       <c r="C20" t="s">
         <v>16</v>
       </c>
       <c r="D20" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>46</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="B21" s="3" t="s">
         <v>54</v>
       </c>
       <c r="C21" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D21" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>46</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="B22" s="3" t="s">
         <v>54</v>
       </c>
       <c r="C22" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D22" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>46</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="B23" s="3" t="s">
         <v>54</v>
       </c>
       <c r="C23" t="s">
@@ -916,311 +1003,316 @@
       <c r="A24" t="s">
         <v>46</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="B24" s="3" t="s">
         <v>54</v>
       </c>
       <c r="C24" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D24" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>46</v>
       </c>
-      <c r="B25" s="4" t="s">
+      <c r="B25" s="3" t="s">
         <v>54</v>
       </c>
       <c r="C25" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D25" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>46</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="B26" s="3" t="s">
         <v>54</v>
       </c>
       <c r="C26" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D26" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>46</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="B27" s="3" t="s">
         <v>54</v>
       </c>
       <c r="C27" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D27" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>46</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>54</v>
+        <v>44</v>
+      </c>
+      <c r="B28" s="3">
+        <v>5</v>
       </c>
       <c r="C28" t="s">
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="D28" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>46</v>
       </c>
-      <c r="B29" s="4" t="s">
+      <c r="B29" s="3" t="s">
         <v>54</v>
       </c>
       <c r="C29" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="D29" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>46</v>
       </c>
-      <c r="B30" s="4" t="s">
+      <c r="B30" s="3" t="s">
         <v>54</v>
       </c>
       <c r="C30" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="D30" t="s">
-        <v>30</v>
+        <v>53</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>46</v>
       </c>
-      <c r="B31" s="4" t="s">
+      <c r="B31" s="3" t="s">
         <v>54</v>
       </c>
       <c r="C31" t="s">
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="D31" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>44</v>
-      </c>
-      <c r="B32" s="4">
-        <v>5</v>
+        <v>46</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>54</v>
       </c>
       <c r="C32" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D32" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>46</v>
-      </c>
-      <c r="B33" s="4" t="s">
-        <v>54</v>
+        <v>44</v>
+      </c>
+      <c r="B33" s="3">
+        <v>5</v>
       </c>
       <c r="C33" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D33" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>44</v>
-      </c>
-      <c r="B34" s="4">
-        <v>5</v>
+        <v>46</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>54</v>
       </c>
       <c r="C34" t="s">
-        <v>34</v>
+        <v>17</v>
       </c>
       <c r="D34" t="s">
-        <v>35</v>
+        <v>14</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>46</v>
-      </c>
-      <c r="B35" s="4" t="s">
-        <v>54</v>
+        <v>44</v>
+      </c>
+      <c r="B35" s="3">
+        <v>4</v>
       </c>
       <c r="C35" t="s">
-        <v>34</v>
+        <v>17</v>
       </c>
       <c r="D35" t="s">
-        <v>37</v>
+        <v>55</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>46</v>
-      </c>
-      <c r="B36" s="4" t="s">
-        <v>54</v>
+        <v>44</v>
+      </c>
+      <c r="B36" s="3">
+        <v>2</v>
       </c>
       <c r="C36" t="s">
-        <v>34</v>
+        <v>17</v>
       </c>
       <c r="D36" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>46</v>
       </c>
-      <c r="B37" s="4" t="s">
+      <c r="B37" s="3" t="s">
         <v>54</v>
       </c>
       <c r="C37" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="D37" t="s">
-        <v>38</v>
+        <v>11</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>46</v>
       </c>
-      <c r="B38" s="4" t="s">
+      <c r="B38" s="3" t="s">
         <v>54</v>
       </c>
       <c r="C38" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="D38" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>44</v>
-      </c>
-      <c r="B39" s="4">
-        <v>5</v>
+        <v>46</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>54</v>
       </c>
       <c r="C39" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="D39" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>44</v>
-      </c>
-      <c r="B40" s="4">
-        <v>4</v>
+        <v>46</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>54</v>
       </c>
       <c r="C40" t="s">
-        <v>41</v>
+        <v>22</v>
       </c>
       <c r="D40" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>44</v>
-      </c>
-      <c r="B41" s="4">
-        <v>3</v>
+        <v>46</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>54</v>
       </c>
       <c r="C41" t="s">
-        <v>41</v>
+        <v>15</v>
       </c>
       <c r="D41" t="s">
-        <v>43</v>
+        <v>10</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>46</v>
       </c>
-      <c r="B42" s="4" t="s">
+      <c r="B42" s="3" t="s">
         <v>54</v>
       </c>
       <c r="C42" t="s">
-        <v>41</v>
+        <v>15</v>
       </c>
       <c r="D42" t="s">
-        <v>45</v>
+        <v>11</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>44</v>
-      </c>
-      <c r="B43" s="4">
-        <v>4</v>
+        <v>46</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>54</v>
       </c>
       <c r="C43" t="s">
-        <v>41</v>
+        <v>15</v>
       </c>
       <c r="D43" t="s">
-        <v>47</v>
+        <v>12</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>46</v>
-      </c>
-      <c r="B44" s="4" t="s">
-        <v>54</v>
+        <v>44</v>
+      </c>
+      <c r="B44" s="3">
+        <v>4</v>
       </c>
       <c r="C44" t="s">
-        <v>41</v>
+        <v>15</v>
       </c>
       <c r="D44" t="s">
-        <v>48</v>
+        <v>13</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>46</v>
       </c>
-      <c r="B45" s="4" t="s">
+      <c r="B45" s="3" t="s">
         <v>54</v>
       </c>
       <c r="C45" t="s">
-        <v>41</v>
+        <v>15</v>
       </c>
       <c r="D45" t="s">
-        <v>49</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A2:D45" xr:uid="{5B0B970C-CDD1-4F7E-94EE-E3839C10F8E5}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:D45">
+      <sortCondition ref="C2:C45"/>
+    </sortState>
+  </autoFilter>
   <mergeCells count="1">
     <mergeCell ref="A1:D1"/>
   </mergeCells>
@@ -1231,12 +1323,411 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{765D9CDE-2ACC-4300-AB58-DC0F6A745C84}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="5" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="65.5703125" style="4" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+    </row>
+    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7" s="9">
+        <v>5</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B11" s="9">
+        <v>4</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B12" s="9">
+        <v>4</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B13" s="9">
+        <v>4</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B14" s="9">
+        <v>3</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B16" s="9">
+        <v>4</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B21" s="9">
+        <v>5</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B27" s="9">
+        <v>3</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B28" s="9">
+        <v>3</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:D1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>